<commit_message>
Edited Excel report 7 sec to generate report now
</commit_message>
<xml_diff>
--- a/AllTags.xlsx
+++ b/AllTags.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Willi\Desktop\CS481\TARGEST.Final-1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{72F5989F-35A6-4855-93A3-3DA883D32BEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{46B5BD42-2F51-4576-8E0E-9C4DB0C9F423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="15" yWindow="15" windowWidth="19185" windowHeight="10065" xr2:uid="{9FA27609-7E1A-4DB7-BE83-7D9EC8D6298C}"/>
+    <workbookView xWindow="15" yWindow="15" windowWidth="19185" windowHeight="10065" xr2:uid="{5C129DF8-9EDA-4FC9-9865-AD7139B1D78F}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -1137,7 +1137,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5CECF9F-E4A4-4F06-AA58-746BE0D5E2C5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D32F2BE7-FD64-4F14-9377-6D9F4ABF11AC}">
   <dimension ref="A1:R418"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Added new Relationship three excel report
</commit_message>
<xml_diff>
--- a/AllTags.xlsx
+++ b/AllTags.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Willi\Desktop\CS481\TARGEST.Final-1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{46B5BD42-2F51-4576-8E0E-9C4DB0C9F423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D434CCFB-DE4D-4BA6-B713-33D161511F12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="15" windowWidth="19185" windowHeight="10065" xr2:uid="{5C129DF8-9EDA-4FC9-9865-AD7139B1D78F}"/>
+    <workbookView minimized="1" xWindow="15" yWindow="15" windowWidth="19185" windowHeight="10065" xr2:uid="{354CD1AA-E8D1-455C-9263-1A27CF8B7A07}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="241">
   <si>
     <t>[PUMP:HRS:100]</t>
   </si>
@@ -1137,7 +1137,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D32F2BE7-FD64-4F14-9377-6D9F4ABF11AC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A486E13C-3559-4257-9F66-AD8A6769B05E}">
   <dimension ref="A1:R418"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -1796,6 +1796,12 @@
       <c r="B40" t="s">
         <v>22</v>
       </c>
+      <c r="H40">
+        <v>38</v>
+      </c>
+      <c r="I40" t="s">
+        <v>199</v>
+      </c>
       <c r="K40">
         <v>38</v>
       </c>
@@ -1804,6 +1810,12 @@
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="H41">
+        <v>39</v>
+      </c>
+      <c r="I41" t="s">
+        <v>200</v>
+      </c>
       <c r="K41">
         <v>39</v>
       </c>
@@ -1812,6 +1824,12 @@
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="H42">
+        <v>40</v>
+      </c>
+      <c r="I42" t="s">
+        <v>201</v>
+      </c>
       <c r="K42">
         <v>40</v>
       </c>
@@ -1823,6 +1841,12 @@
       <c r="A43" t="s">
         <v>23</v>
       </c>
+      <c r="H43">
+        <v>41</v>
+      </c>
+      <c r="I43" t="s">
+        <v>202</v>
+      </c>
       <c r="K43">
         <v>41</v>
       </c>
@@ -1834,6 +1858,12 @@
       <c r="B44" t="s">
         <v>24</v>
       </c>
+      <c r="H44">
+        <v>42</v>
+      </c>
+      <c r="I44" t="s">
+        <v>203</v>
+      </c>
       <c r="K44">
         <v>42</v>
       </c>
@@ -1842,6 +1872,12 @@
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="H45">
+        <v>43</v>
+      </c>
+      <c r="I45" t="s">
+        <v>204</v>
+      </c>
       <c r="K45">
         <v>43</v>
       </c>
@@ -1850,6 +1886,12 @@
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="H46">
+        <v>44</v>
+      </c>
+      <c r="I46" t="s">
+        <v>205</v>
+      </c>
       <c r="K46">
         <v>44</v>
       </c>
@@ -1861,6 +1903,12 @@
       <c r="A47" t="s">
         <v>25</v>
       </c>
+      <c r="H47">
+        <v>45</v>
+      </c>
+      <c r="I47" t="s">
+        <v>206</v>
+      </c>
       <c r="K47">
         <v>45</v>
       </c>
@@ -1872,6 +1920,12 @@
       <c r="B48" t="s">
         <v>26</v>
       </c>
+      <c r="H48">
+        <v>46</v>
+      </c>
+      <c r="I48" t="s">
+        <v>207</v>
+      </c>
       <c r="K48">
         <v>46</v>
       </c>
@@ -1880,6 +1934,12 @@
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="H49">
+        <v>47</v>
+      </c>
+      <c r="I49" t="s">
+        <v>208</v>
+      </c>
       <c r="K49">
         <v>47</v>
       </c>
@@ -1888,6 +1948,12 @@
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="H50">
+        <v>48</v>
+      </c>
+      <c r="I50" t="s">
+        <v>209</v>
+      </c>
       <c r="K50">
         <v>48</v>
       </c>
@@ -1899,6 +1965,12 @@
       <c r="A51" t="s">
         <v>27</v>
       </c>
+      <c r="H51">
+        <v>49</v>
+      </c>
+      <c r="I51" t="s">
+        <v>210</v>
+      </c>
       <c r="K51">
         <v>49</v>
       </c>
@@ -1910,6 +1982,12 @@
       <c r="B52" t="s">
         <v>28</v>
       </c>
+      <c r="H52">
+        <v>50</v>
+      </c>
+      <c r="I52" t="s">
+        <v>211</v>
+      </c>
       <c r="K52">
         <v>50</v>
       </c>
@@ -1918,11 +1996,25 @@
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="H53">
+        <v>51</v>
+      </c>
+      <c r="I53" t="s">
+        <v>212</v>
+      </c>
       <c r="K53">
         <v>51</v>
       </c>
       <c r="L53" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="H54">
+        <v>52</v>
+      </c>
+      <c r="I54" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.45">

</xml_diff>